<commit_message>
update base line test result
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47476221-220F-46EC-8D11-E644C324BFCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4BD96F-65E2-40D6-B241-C74E2F772A44}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>BaseLine</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>attack from (-1,1) L2</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>X-115</t>
   </si>
 </sst>
 </file>
@@ -376,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:E15"/>
+  <dimension ref="B3:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K14:K15"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,6 +402,9 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
@@ -421,106 +430,114 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>6.3600000000000004E-2</v>
-      </c>
-      <c r="D6">
-        <v>0.1273</v>
-      </c>
-      <c r="E6">
-        <v>0.32729999999999998</v>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>0.1996</v>
+        <v>6.3600000000000004E-2</v>
       </c>
       <c r="D7">
-        <v>156.28229999999999</v>
-      </c>
-      <c r="E7">
-        <v>156.28219999999999</v>
+        <v>0.91820000000000002</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>0.1996</v>
+      </c>
+      <c r="D8">
+        <v>0.20780000000000001</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>1.8200000000000001E-2</v>
-      </c>
-      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>1.8200000000000001E-2</v>
-      </c>
-      <c r="E10" t="s">
+        <v>0.20910000000000001</v>
+      </c>
+      <c r="D10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>0.30909999999999999</v>
+      </c>
+      <c r="E11" t="s">
         <v>10</v>
-      </c>
-      <c r="D11">
-        <v>0.34549999999999997</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <v>25.35</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
       </c>
       <c r="D13">
-        <v>0.59089999999999998</v>
+        <v>0.34549999999999997</v>
+      </c>
+      <c r="E13">
+        <v>0.38179999999999997</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
         <v>10</v>
+      </c>
+      <c r="D14">
+        <v>25.35</v>
+      </c>
+      <c r="E14">
+        <v>25.37</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>0.59089999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>9</v>
       </c>
-      <c r="D15">
+      <c r="D17">
         <v>0.61819999999999997</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Attack baseline V2 +MIM support
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -3,12 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4BD96F-65E2-40D6-B241-C74E2F772A44}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8580CC57-DF82-4AB2-ABFB-2837B46E1C85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="play" sheetId="1" r:id="rId1"/>
+    <sheet name="test result" sheetId="3" r:id="rId2"/>
+    <sheet name="Methods" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="75">
   <si>
     <t>BaseLine</t>
   </si>
@@ -65,19 +67,214 @@
   </si>
   <si>
     <t>X-115</t>
+  </si>
+  <si>
+    <t>eps = 1/255</t>
+  </si>
+  <si>
+    <t>0.51,  0.0065</t>
+  </si>
+  <si>
+    <t>FGSM</t>
+  </si>
+  <si>
+    <t>L-BFGS</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Targeted</t>
+  </si>
+  <si>
+    <t>inf, 1,2</t>
+  </si>
+  <si>
+    <t>One Shot</t>
+  </si>
+  <si>
+    <t>Inf</t>
+  </si>
+  <si>
+    <t>BIM &amp; ILCM</t>
+  </si>
+  <si>
+    <t>Non-Targeted</t>
+  </si>
+  <si>
+    <t>Iterative</t>
+  </si>
+  <si>
+    <t>MIM</t>
+  </si>
+  <si>
+    <t>JSMA</t>
+  </si>
+  <si>
+    <t>One-pixel</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>CW</t>
+  </si>
+  <si>
+    <t>DeepFool</t>
+  </si>
+  <si>
+    <t>Uni.perturbations</t>
+  </si>
+  <si>
+    <t>UPSET</t>
+  </si>
+  <si>
+    <t>ANGRI</t>
+  </si>
+  <si>
+    <t>Houdini</t>
+  </si>
+  <si>
+    <t>ATNs</t>
+  </si>
+  <si>
+    <t>Inf,0,2</t>
+  </si>
+  <si>
+    <t>Inf,2</t>
+  </si>
+  <si>
+    <t>Box-constrained,  mini preturbations</t>
+  </si>
+  <si>
+    <t>[80] ‘one-step target class’</t>
+  </si>
+  <si>
+    <t>L0, limit pixels to change</t>
+  </si>
+  <si>
+    <t>attack distillation method. Transfer!</t>
+  </si>
+  <si>
+    <t>for all images,  not for specific</t>
+  </si>
+  <si>
+    <t>universal</t>
+  </si>
+  <si>
+    <t>train network, heavy?</t>
+  </si>
+  <si>
+    <t>ElasticNetMethod</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1709.04114</t>
+  </si>
+  <si>
+    <t>MadryEtAl</t>
+  </si>
+  <si>
+    <t>MaxConfidence</t>
+  </si>
+  <si>
+    <t>MomentumIterativeMethod</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/1710.06081.pdf</t>
+  </si>
+  <si>
+    <t>2017 won</t>
+  </si>
+  <si>
+    <t>SPSA</t>
+  </si>
+  <si>
+    <t>gridient free</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1802.05666</t>
+  </si>
+  <si>
+    <t>SaliencyMapMethod</t>
+  </si>
+  <si>
+    <t>Semantic</t>
+  </si>
+  <si>
+    <t>VirtualAdversarialMethod</t>
+  </si>
+  <si>
+    <t>0,  20.32</t>
+  </si>
+  <si>
+    <t>attack model</t>
+  </si>
+  <si>
+    <t>params</t>
+  </si>
+  <si>
+    <t>incpetion_v1</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>FGM</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>acc</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>Transfer to Inception_v1</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>Transfer to resnet_v1_50</t>
+  </si>
+  <si>
+    <t>Transfer to vgg_16</t>
+  </si>
+  <si>
+    <t>32/255</t>
+  </si>
+  <si>
+    <t>resnet_v1_50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -97,13 +294,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -382,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:E17"/>
+  <dimension ref="B3:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,8 +742,540 @@
         <v>0.61819999999999997</v>
       </c>
     </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31AF996-4C64-44D3-BDB6-FE7C90CA3110}">
+  <dimension ref="B2:K6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3">
+        <v>6.3600000000000004E-2</v>
+      </c>
+      <c r="G3">
+        <v>25.44</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="K3">
+        <v>0.309</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>20.32</v>
+      </c>
+      <c r="H4">
+        <v>389</v>
+      </c>
+      <c r="J4">
+        <v>0.191</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0.96360000000000001</v>
+      </c>
+      <c r="G5">
+        <v>4.4699999999999997E-2</v>
+      </c>
+      <c r="H5">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>0.43640000000000001</v>
+      </c>
+      <c r="G6">
+        <v>22.21</v>
+      </c>
+      <c r="H6">
+        <v>962</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20D29FC0-70F8-45D4-A595-DC52422B7199}">
+  <dimension ref="A2:H29"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="38" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H9" r:id="rId1" xr:uid="{BB42DDD5-9864-44FA-BDEF-F6843D3CE63A}"/>
+    <hyperlink ref="H12" r:id="rId2" xr:uid="{5BF16318-7EBE-4492-9F85-C85DA5952553}"/>
+    <hyperlink ref="H13" r:id="rId3" xr:uid="{9FDF7D18-4CA1-4EBD-906F-BC4F9CF876E1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
V6 + SGMIM +Embedded Models
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8580CC57-DF82-4AB2-ABFB-2837B46E1C85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150C3617-C0B5-4E5D-9729-1ECA4DE93FB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,18 +11,24 @@
     <sheet name="play" sheetId="1" r:id="rId1"/>
     <sheet name="test result" sheetId="3" r:id="rId2"/>
     <sheet name="Methods" sheetId="2" r:id="rId3"/>
+    <sheet name="Inspire" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="85">
   <si>
     <t>BaseLine</t>
   </si>
@@ -210,9 +216,6 @@
     <t>attack model</t>
   </si>
   <si>
-    <t>params</t>
-  </si>
-  <si>
     <t>incpetion_v1</t>
   </si>
   <si>
@@ -243,10 +246,43 @@
     <t>Transfer to vgg_16</t>
   </si>
   <si>
-    <t>32/255</t>
-  </si>
-  <si>
     <t>resnet_v1_50</t>
+  </si>
+  <si>
+    <t>eps_radio</t>
+  </si>
+  <si>
+    <t>inter</t>
+  </si>
+  <si>
+    <t>preprocess</t>
+  </si>
+  <si>
+    <t>(-1,1)</t>
+  </si>
+  <si>
+    <t>ATN</t>
+  </si>
+  <si>
+    <t>reduce computational cost at test stage</t>
+  </si>
+  <si>
+    <t>Ghost Network</t>
+  </si>
+  <si>
+    <t>More ghost network to improve IGSM</t>
+  </si>
+  <si>
+    <t>SGMIM</t>
+  </si>
+  <si>
+    <t>Embedd 3</t>
+  </si>
+  <si>
+    <t>0,255</t>
+  </si>
+  <si>
+    <t>batch</t>
   </si>
 </sst>
 </file>
@@ -277,12 +313,18 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -298,10 +340,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -766,155 +810,485 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31AF996-4C64-44D3-BDB6-FE7C90CA3110}">
-  <dimension ref="B2:K6"/>
+  <dimension ref="B2:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="8" width="9.5703125" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>61</v>
       </c>
       <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>62</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3">
+        <v>110</v>
+      </c>
+      <c r="E3">
+        <f>(32/255)/2</f>
+        <v>6.2745098039215685E-2</v>
+      </c>
+      <c r="F3" t="s">
         <v>64</v>
       </c>
-      <c r="E2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H2" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>6.3600000000000004E-2</v>
+      </c>
+      <c r="J3">
+        <v>25.44</v>
+      </c>
+      <c r="L3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="N3">
+        <v>0.309</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4">
+        <v>110</v>
+      </c>
+      <c r="E4">
+        <f>(32/255)/2</f>
+        <v>6.2745098039215685E-2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>20.32</v>
+      </c>
+      <c r="K4">
+        <v>389</v>
+      </c>
+      <c r="M4">
+        <v>0.191</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5">
+        <v>110</v>
+      </c>
+      <c r="E5">
+        <f>(32/255)/2</f>
+        <v>6.2745098039215685E-2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>20</v>
+      </c>
+      <c r="I5">
+        <v>0.96360000000000001</v>
+      </c>
+      <c r="J5">
+        <v>4.4699999999999997E-2</v>
+      </c>
+      <c r="K5">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6">
+        <v>110</v>
+      </c>
+      <c r="E6">
+        <f>(32/255)/2</f>
+        <v>6.2745098039215685E-2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
         <v>23</v>
       </c>
-      <c r="F3">
-        <v>6.3600000000000004E-2</v>
-      </c>
-      <c r="G3">
-        <v>25.44</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="H6">
+        <v>20</v>
+      </c>
+      <c r="I6">
+        <v>0.43640000000000001</v>
+      </c>
+      <c r="J6">
+        <v>22.21</v>
+      </c>
+      <c r="K6">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7">
+        <v>110</v>
+      </c>
+      <c r="E7">
+        <v>0.1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7">
+        <v>20</v>
+      </c>
+      <c r="I7">
+        <v>0.191</v>
+      </c>
+      <c r="J7">
+        <v>31.23</v>
+      </c>
+      <c r="K7">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8">
+        <v>-115</v>
+      </c>
+      <c r="D8">
+        <v>110</v>
+      </c>
+      <c r="E8">
+        <v>0.1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8">
+        <v>20</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>32.32</v>
+      </c>
+      <c r="K8">
+        <v>961</v>
+      </c>
+      <c r="L8">
+        <v>0.2636</v>
+      </c>
+      <c r="M8" t="s">
         <v>10</v>
       </c>
-      <c r="J3">
-        <v>0.20899999999999999</v>
-      </c>
-      <c r="K3">
-        <v>0.309</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="N8">
+        <v>0.28189999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9">
+        <v>110</v>
+      </c>
+      <c r="E9">
+        <v>0.1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>5.45E-2</v>
+      </c>
+      <c r="J9">
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10">
+        <v>110</v>
+      </c>
+      <c r="E10">
+        <v>0.1</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>12.28</v>
+      </c>
+      <c r="K10">
+        <v>210</v>
+      </c>
+      <c r="M10">
+        <v>0.1636</v>
+      </c>
+      <c r="N10">
+        <v>0.254</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11">
+        <v>110</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="F11" t="s">
         <v>27</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G11" t="s">
         <v>23</v>
       </c>
-      <c r="F4">
+      <c r="H11" s="3">
+        <v>5</v>
+      </c>
+      <c r="I11">
         <v>0</v>
       </c>
-      <c r="G4">
-        <v>20.32</v>
-      </c>
-      <c r="H4">
-        <v>389</v>
-      </c>
-      <c r="J4">
-        <v>0.191</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="J11">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12">
+        <v>110</v>
+      </c>
+      <c r="E12">
+        <v>0.1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="3">
+        <v>100</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>13.97</v>
+      </c>
+      <c r="K12">
+        <v>2010.9</v>
+      </c>
+      <c r="M12">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="N12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13">
+        <v>50</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F13" t="s">
         <v>27</v>
       </c>
-      <c r="E5">
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13">
         <v>2</v>
       </c>
-      <c r="F5">
-        <v>0.96360000000000001</v>
-      </c>
-      <c r="G5">
-        <v>4.4699999999999997E-2</v>
-      </c>
-      <c r="H5">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="J13">
+        <v>3.56</v>
+      </c>
+      <c r="K13">
+        <v>200</v>
+      </c>
+      <c r="L13">
+        <v>0.2</v>
+      </c>
+      <c r="M13">
+        <v>0.18</v>
+      </c>
+      <c r="N13">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14">
+        <v>50</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="F14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" t="s">
         <v>23</v>
       </c>
-      <c r="F6">
-        <v>0.43640000000000001</v>
-      </c>
-      <c r="G6">
-        <v>22.21</v>
-      </c>
-      <c r="H6">
-        <v>962</v>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>1.996</v>
+      </c>
+      <c r="L14">
+        <v>0.3</v>
+      </c>
+      <c r="M14">
+        <v>0.24</v>
+      </c>
+      <c r="N14">
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>
@@ -927,7 +1301,7 @@
   <dimension ref="A2:H29"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,4 +1652,39 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8256FD00-8941-42ED-8238-21974BCCED96}">
+  <dimension ref="B2:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="65.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Batch Predict on GPU
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EAEDF0-9AD7-433C-8C9B-2906E7B06311}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB903D4E-BF18-4A81-BA05-799D31A4AE45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="101">
   <si>
     <t>BaseLine</t>
   </si>
@@ -307,13 +307,31 @@
     <t>MSB defense</t>
   </si>
   <si>
-    <t>!!!!!</t>
-  </si>
-  <si>
     <t>224-&gt;299</t>
   </si>
   <si>
-    <t>input resize ratio</t>
+    <t>random distort</t>
+  </si>
+  <si>
+    <t>anti training</t>
+  </si>
+  <si>
+    <t>existing models to transfer learning</t>
+  </si>
+  <si>
+    <t>to many similar inputs,  and average classifier</t>
+  </si>
+  <si>
+    <t>!!!!!  Use this example to train.</t>
+  </si>
+  <si>
+    <t>input resize keep ratio</t>
+  </si>
+  <si>
+    <t>get adv training datasets</t>
+  </si>
+  <si>
+    <t>augment,  MIM output, MSB</t>
   </si>
 </sst>
 </file>
@@ -1804,10 +1822,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8256FD00-8941-42ED-8238-21974BCCED96}">
-  <dimension ref="B2:D12"/>
+  <dimension ref="B2:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1857,7 +1875,23 @@
         <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1867,25 +1901,34 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA365D85-EB91-403E-B758-0FD479EA1FC0}">
-  <dimension ref="B2:B3"/>
+  <dimension ref="B2:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>94</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix batch Attack issue
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB903D4E-BF18-4A81-BA05-799D31A4AE45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672CDBF1-002E-44BB-A9E8-2BA59A8E505B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="play" sheetId="1" r:id="rId1"/>
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31AF996-4C64-44D3-BDB6-FE7C90CA3110}">
   <dimension ref="B2:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1903,7 +1903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA365D85-EB91-403E-B758-0FD479EA1FC0}">
   <dimension ref="B2:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Data Cleanup 1. split good and bad 2. convert good into adv
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672CDBF1-002E-44BB-A9E8-2BA59A8E505B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40045B28-10F0-42C0-85C6-8867FD008F1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="play" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="102">
   <si>
     <t>BaseLine</t>
   </si>
@@ -332,6 +332,9 @@
   </si>
   <si>
     <t>augment,  MIM output, MSB</t>
+  </si>
+  <si>
+    <t>dropout pixels</t>
   </si>
 </sst>
 </file>
@@ -861,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31AF996-4C64-44D3-BDB6-FE7C90CA3110}">
   <dimension ref="B2:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1822,10 +1825,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8256FD00-8941-42ED-8238-21974BCCED96}">
-  <dimension ref="B2:D14"/>
+  <dimension ref="B2:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1892,6 +1895,11 @@
       </c>
       <c r="C14" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>